<commit_message>
"data binding changed to data file"
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KatalonStudio\DemoProj\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saranya/Desktop/DemoProj/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947D29AA-3973-4284-94FC-1BAD3CFA38A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302603D5-E900-4E4B-8F97-A44A419EBAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="954" xr2:uid="{C6F85985-84AE-4DCB-8550-9B2F16782E4E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19420" windowHeight="10420" tabRatio="954" xr2:uid="{C6F85985-84AE-4DCB-8550-9B2F16782E4E}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Test case to verify username and password with special chars</t>
+  </si>
+  <si>
+    <t>p8rFjx5pgvU=</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
@@ -497,18 +500,20 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="1"/>
+    <col min="2" max="2" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -522,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -536,7 +541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -550,7 +555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -562,7 +567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -574,7 +579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -584,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -592,13 +597,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -612,7 +617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>